<commit_message>
Added Product Type menu, sheet, dropdown.
</commit_message>
<xml_diff>
--- a/RPMS/Configuration.xlsx
+++ b/RPMS/Configuration.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
     <sheet name="Tax" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductType" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Product Name</t>
   </si>
@@ -98,6 +99,36 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>9cdbd0c4-8435-4848-9732-c6545ee41faa</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>15.5</t>
+  </si>
+  <si>
+    <t>5/8/2019 8:53:31 PM</t>
+  </si>
+  <si>
+    <t>9aae78bb-0d58-49cb-b91e-25b5d43d60c1</t>
+  </si>
+  <si>
+    <t>Service Tax</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>5/8/2019 8:54:03 PM</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>Key</t>
   </si>
 </sst>
 </file>
@@ -515,10 +546,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +571,75 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Synced latest from Master.
</commit_message>
<xml_diff>
--- a/RPMS/Configuration.xlsx
+++ b/RPMS/Configuration.xlsx
@@ -378,10 +378,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -390,7 +390,7 @@
     <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row spans="1:7" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -413,27 +413,78 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
+    <row spans="1:7" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>d0f46e1e-20f5-431f-8a56-48e84b657f8c</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Name Kumar1</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>SKUN0</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Code0</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Desc0</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>5/9/2019 9:40:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>49cd1269-d104-4a11-9985-561a807f6c64</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Product2</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>SKU2</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>Code2</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Desc2</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>5/9/2019 9:40:28 PM</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>